<commit_message>
completed docs for lab2
</commit_message>
<xml_diff>
--- a/docs/lab2/Lab02_Review Report.xlsx
+++ b/docs/lab2/Lab02_Review Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.bertici\Uni\verificare-si-testare\bsci0283\docs\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C2F933-4210-439B-BAE1-D17584457C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74577F46-26F5-415D-B6D1-17FD49FD3D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2160" windowWidth="19176" windowHeight="10176" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -1449,7 +1449,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1744,7 +1744,9 @@
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1766,8 +1768,8 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1860,7 +1862,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="20">
         <f>B10+1</f>
         <v>2</v>
@@ -2165,7 +2167,9 @@
       </c>
       <c r="D32" s="35"/>
       <c r="E32" s="35"/>
-      <c r="F32" s="22"/>
+      <c r="F32" s="22">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>